<commit_message>
more changes to code
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template.xlsx
+++ b/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">General Empty</t>
   </si>
   <si>
-    <t xml:space="preserve">smart_attribute</t>
+    <t xml:space="preserve">smart_attribute_state</t>
   </si>
   <si>
     <t xml:space="preserve">additional display</t>
@@ -259,15 +259,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
add tests session level etc
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template.xlsx
+++ b/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">smart_attribute_state</t>
   </si>
   <si>
-    <t xml:space="preserve">additional display</t>
+    <t xml:space="preserve">additional display,stock</t>
   </si>
 </sst>
 </file>
@@ -259,14 +259,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
processing exclusion template on kpi lvl for sos vs target
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template.xlsx
+++ b/Projects/PEPSICOUK/Data/Inclusion_Exclusion_Template.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="exclusion_rules" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="store_policy" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -58,7 +59,37 @@
     <t xml:space="preserve">smart_attribute_state</t>
   </si>
   <si>
-    <t xml:space="preserve">additional display,stock</t>
+    <t xml:space="preserve">additional display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hero SKU Space to Sales Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brand_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLACK COUNTRY SNACKS, AKSAM PALUSZKI, LAJKONIK PALUSZKI, ALKA ELEPHANT, RUMPLERS, TABITHA, CHEF'S LARDER, BOROMIR, COFRESH, JIFFY POP, CROCO, THE CURATORS, FRESHERS, FUDCO, GEFEN, GINNI'S, OH MY GURU!, HALDIRAMS, HALDIRAMS SNACKS, INDIE BAY SNACKS, INNATE, JACK-LNK'S, EAZY-PP-PPCRN, ZWEIFEL CRISPS, HUNKY DORYS CRISPS, LAJKONIK JUNIOR, LOVE CHIN CHIN, NISHAS SNACKS, NUTELLA, OSEM SAVOURY SNACK, OUR LITTLE REBELL!ON, EPIC, CRAWFORDS, FLIPZ, OATIS, RYMUT SNACKS, GINCO, SUNSHINE SNACKS, JAY'S, MIDLAND SNACKS, RED MILL SAVOURY SNACKS, SENSIBLE PORTIONS, VISCONTI SNACKS, WELL &amp; TRULY SNACKS, WILD WEST, WILDING'S, BLUE DRAGON, BEPPS, BLUE DIAMOND, COFRESH SNACKS, SCHAR, OLD EL PASO, PLANTERS, LINWOODS, CYPRESSA, KOHINOOR SNACKS, KOIKEYA, PALUSZKI, LORENZ CRISPS, MCCOLGAN, ITSU, NAIRNS, NATURES STORE SNACKS, NIM'S, BAMBA SNACKS, BISSLI SNACKS, SHARWOODS, MR PORKY SNACKS, TYGRYSKI, THE REAL PORK CRACKLING CO SNACKS, THE SNAFFLING PIG CO, WHITWORTHS, YUM &amp; YAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand Space to Sales Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub Brand Space to Sales Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PepsiCo Segment Space to Sales Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PepsiCo Sub Segment Space to Sales Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">additional_attribute_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TT</t>
   </si>
 </sst>
 </file>
@@ -154,7 +185,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,6 +208,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -256,18 +295,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.71255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.2024291497976"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -326,6 +368,77 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -335,4 +448,85 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>